<commit_message>
adding yearsOf, getting 100% in RF
</commit_message>
<xml_diff>
--- a/1-data-understanding/1-input/support/homeworking/homeworking.xlsx
+++ b/1-data-understanding/1-input/support/homeworking/homeworking.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\hrms-gys\hrms-gys-ml\1-data-understanding\1-input\support\homeworking-pdf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\hrms-gys\hrms-gys-ml\1-data-understanding\1-input\support\homeworking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F972FB-25C7-4EA5-AEC2-59C5815D9CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18718A97-1897-4E45-A064-E5C0AAF1E63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="265">
   <si>
     <t>Juan</t>
   </si>
@@ -808,6 +808,30 @@
   </si>
   <si>
     <t>Cuadros</t>
+  </si>
+  <si>
+    <t>Teodoro</t>
+  </si>
+  <si>
+    <t>Enrique</t>
+  </si>
+  <si>
+    <t>Zapata</t>
+  </si>
+  <si>
+    <t>Luyo</t>
+  </si>
+  <si>
+    <t>Ever</t>
+  </si>
+  <si>
+    <t>Yalico</t>
+  </si>
+  <si>
+    <t>Angeli</t>
+  </si>
+  <si>
+    <t>Velasquez</t>
   </si>
 </sst>
 </file>
@@ -872,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -881,6 +905,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1164,12 +1194,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13883A-6976-4FDD-BF62-8F22C76FC29D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I2" sqref="I1:I1048576"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,11 +1712,15 @@
       <c r="A38" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="C38" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -2259,6 +2293,40 @@
       <c r="D80" s="3" t="s">
         <v>139</v>
       </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D39" xr:uid="{AE13883A-6976-4FDD-BF62-8F22C76FC29D}"/>

</xml_diff>

<commit_message>
running for 0.85 sensitivity
</commit_message>
<xml_diff>
--- a/1-data-understanding/1-input/support/homeworking/homeworking.xlsx
+++ b/1-data-understanding/1-input/support/homeworking/homeworking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\hrms-gys\hrms-gys-ml\1-data-understanding\1-input\support\homeworking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905A74D2-6DB0-4763-8515-F63DF9808C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4661EB8-7D2B-40F2-8EB1-CF2A7C9875FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="305">
   <si>
     <t>Juan</t>
   </si>
@@ -856,6 +856,102 @@
   </si>
   <si>
     <t>Bernuy</t>
+  </si>
+  <si>
+    <t>Alberto</t>
+  </si>
+  <si>
+    <t>Sotelo</t>
+  </si>
+  <si>
+    <t>Cordero</t>
+  </si>
+  <si>
+    <t>Edwin</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Fernandez</t>
+  </si>
+  <si>
+    <t>Jazmin</t>
+  </si>
+  <si>
+    <t>Regalado</t>
+  </si>
+  <si>
+    <t>Cabello</t>
+  </si>
+  <si>
+    <t>Percy</t>
+  </si>
+  <si>
+    <t>Aguilar</t>
+  </si>
+  <si>
+    <t>Marin</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Gianfranco</t>
+  </si>
+  <si>
+    <t>Avalos</t>
+  </si>
+  <si>
+    <t>Cristobal</t>
+  </si>
+  <si>
+    <t>Guillermo</t>
+  </si>
+  <si>
+    <t>Sandoval</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Joaquin</t>
+  </si>
+  <si>
+    <t>Guillen</t>
+  </si>
+  <si>
+    <t>Huarcaya</t>
+  </si>
+  <si>
+    <t>Arguedas</t>
+  </si>
+  <si>
+    <t>Quiñonez</t>
+  </si>
+  <si>
+    <t>Danmert</t>
+  </si>
+  <si>
+    <t>Jonelly</t>
+  </si>
+  <si>
+    <t>Costilla</t>
+  </si>
+  <si>
+    <t>Claros</t>
+  </si>
+  <si>
+    <t>Rodail</t>
+  </si>
+  <si>
+    <t>Rugel</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Reyes</t>
   </si>
 </sst>
 </file>
@@ -920,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -929,12 +1025,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1218,12 +1308,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13883A-6976-4FDD-BF62-8F22C76FC29D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I2" sqref="I1:I1048576"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2399,10 +2489,150 @@
       <c r="D86" s="3"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
+      <c r="A87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B89" s="1"/>
+      <c r="C89" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B90" s="1"/>
+      <c r="C90" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B94" s="1"/>
+      <c r="C94" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B96" s="1"/>
+      <c r="C96" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>304</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D40" xr:uid="{AE13883A-6976-4FDD-BF62-8F22C76FC29D}"/>

</xml_diff>